<commit_message>
changes about test outputs
</commit_message>
<xml_diff>
--- a/scoring/forms/JPSDI/JPSDI93_test_2.xlsx
+++ b/scoring/forms/JPSDI/JPSDI93_test_2.xlsx
@@ -10,6 +10,7 @@
     <sheet name="question_answers" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="outputs" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="outputs1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="outputs2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -623,7 +624,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -633,7 +634,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -643,7 +644,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -653,18 +654,18 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>sath_tahavol_ravani_fard</t>
+          <t>psdi</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>level_3,</t>
+          <t>level_1,level_4</t>
         </is>
       </c>
     </row>
@@ -689,4 +690,22 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>